<commit_message>
fix stopu issue seet 업로드
</commit_message>
<xml_diff>
--- a/교사팀_기능명세서.xlsx
+++ b/교사팀_기능명세서.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyg51\Desktop\car_accident\VIEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21\Desktop\car\VIEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C5171E-6283-4694-A053-0CEFC2839DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15615" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="기능명세서" sheetId="1" r:id="rId1"/>
+    <sheet name="issue" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">기능명세서!$A$2:$J$25</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>대분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -270,17 +270,77 @@
   </si>
   <si>
     <t>HTML 및 CSS 점검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">git 협업툴 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발생일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해결일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해결방안</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>issue관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>issue내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가기능 issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>error issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색기능 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객센터 검색기능 및 사고건수, 사망자, 부상자 몇 명 이상의 건수 조회 검색기능 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지유</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>import시 git이 아닌 gradle로 가능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +379,14 @@
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -381,7 +449,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -427,6 +495,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,9 +528,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -749,42 +844,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.25" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.75" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.875" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.25" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.58203125" style="5"/>
-    <col min="10" max="10" width="40.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.58203125" style="5"/>
+    <col min="7" max="9" width="8.625" style="5"/>
+    <col min="10" max="10" width="40.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="44">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="45">
+      <c r="A1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="17"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="35.15" customHeight="1">
+    <row r="2" spans="1:10" ht="35.1" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +912,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -839,7 +934,7 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="15"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="4" t="s">
         <v>44</v>
       </c>
@@ -861,7 +956,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -887,8 +982,8 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -911,8 +1006,8 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="3" t="s">
         <v>34</v>
       </c>
@@ -929,10 +1024,10 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="23" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -953,8 +1048,8 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
@@ -973,8 +1068,8 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
@@ -993,8 +1088,8 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1013,8 +1108,8 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="3" t="s">
         <v>39</v>
       </c>
@@ -1033,10 +1128,10 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="23" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1055,8 +1150,8 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1073,8 +1168,8 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1091,8 +1186,8 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1109,8 +1204,8 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1127,8 +1222,8 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1145,8 +1240,8 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="3" t="s">
         <v>9</v>
       </c>
@@ -1163,7 +1258,7 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="15"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="11" t="s">
         <v>52</v>
       </c>
@@ -1183,10 +1278,10 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="23" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1205,8 +1300,8 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="3" t="s">
         <v>18</v>
       </c>
@@ -1223,8 +1318,8 @@
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1243,8 +1338,8 @@
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="3" t="s">
         <v>20</v>
       </c>
@@ -1261,7 +1356,7 @@
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="15"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="4" t="s">
         <v>55</v>
       </c>
@@ -1281,7 +1376,7 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1303,7 +1398,7 @@
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="15"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="4" t="s">
         <v>58</v>
       </c>
@@ -1323,7 +1418,7 @@
       <c r="J27" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J25" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:J25"/>
   <mergeCells count="14">
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A1:D1"/>
@@ -1343,4 +1438,114 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="11.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="80.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45">
+      <c r="A1" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="21">
+        <v>44735</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="21">
+        <v>44735</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="20">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="21">
+        <v>44735</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix stopu 휴가 추가
</commit_message>
<xml_diff>
--- a/교사팀_기능명세서.xlsx
+++ b/교사팀_기능명세서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyg51\Desktop\car_accident\VIEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37001B2-9A8B-4097-BAB8-4F46B5ADCEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CAEE87-DE75-4EFD-A472-D0EE28250CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="기능명세서" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="164">
   <si>
     <t>대분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -680,6 +680,10 @@
   </si>
   <si>
     <t>휴(정수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-06-28 지유 휴가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1273,7 +1277,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1466,6 +1470,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1485,27 +1522,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1538,34 +1554,25 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1981,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17"/>
@@ -2000,16 +2007,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="44">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="65"/>
+      <c r="F1" s="76"/>
       <c r="G1" s="9" t="s">
         <v>40</v>
       </c>
@@ -2047,7 +2054,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="74" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -2075,7 +2082,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="63"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="21" t="s">
         <v>42</v>
       </c>
@@ -2085,11 +2092,15 @@
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
       <c r="F4" s="7">
         <v>44739</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="7">
+        <v>44739</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="10" t="s">
@@ -2097,7 +2108,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="74" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="22" t="s">
@@ -2123,8 +2134,8 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="63"/>
-      <c r="B6" s="66" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="77" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2147,8 +2158,8 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="63"/>
-      <c r="B7" s="66"/>
+      <c r="A7" s="74"/>
+      <c r="B7" s="77"/>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
@@ -2171,10 +2182,10 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="78" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -2195,17 +2206,17 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="63"/>
-      <c r="B9" s="67"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="7">
-        <v>44740</v>
+        <v>44741</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -2215,8 +2226,8 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="63"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
@@ -2235,8 +2246,8 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="63"/>
-      <c r="B11" s="66" t="s">
+      <c r="A11" s="74"/>
+      <c r="B11" s="77" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -2255,8 +2266,8 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="63"/>
-      <c r="B12" s="66"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
@@ -2275,10 +2286,10 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="79" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -2303,8 +2314,8 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="63"/>
-      <c r="B14" s="69"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2327,8 +2338,8 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="63"/>
-      <c r="B15" s="69"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
@@ -2349,8 +2360,8 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="63"/>
-      <c r="B16" s="69"/>
+      <c r="A16" s="74"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
@@ -2373,8 +2384,8 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="63"/>
-      <c r="B17" s="69"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
@@ -2395,8 +2406,8 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="63"/>
-      <c r="B18" s="69"/>
+      <c r="A18" s="74"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
@@ -2417,8 +2428,8 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="63"/>
-      <c r="B19" s="69"/>
+      <c r="A19" s="74"/>
+      <c r="B19" s="80"/>
       <c r="C19" s="3" t="s">
         <v>9</v>
       </c>
@@ -2439,10 +2450,10 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="77" t="s">
         <v>50</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -2461,8 +2472,8 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="63"/>
-      <c r="B21" s="66"/>
+      <c r="A21" s="74"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="3" t="s">
         <v>17</v>
       </c>
@@ -2479,8 +2490,8 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="63"/>
-      <c r="B22" s="67" t="s">
+      <c r="A22" s="74"/>
+      <c r="B22" s="78" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -2499,8 +2510,8 @@
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="63"/>
-      <c r="B23" s="67"/>
+      <c r="A23" s="74"/>
+      <c r="B23" s="78"/>
       <c r="C23" s="3" t="s">
         <v>19</v>
       </c>
@@ -2517,7 +2528,7 @@
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="63"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="22" t="s">
         <v>51</v>
       </c>
@@ -2537,7 +2548,7 @@
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="74" t="s">
         <v>52</v>
       </c>
       <c r="B25" s="22" t="s">
@@ -2559,7 +2570,7 @@
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="63"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="21" t="s">
         <v>54</v>
       </c>
@@ -2606,7 +2617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -2623,30 +2634,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="44">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="15"/>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="71" t="s">
         <v>68</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="97" t="s">
+      <c r="D2" s="73" t="s">
         <v>57</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="97" t="s">
+      <c r="F2" s="73" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="16" t="s">
@@ -2758,7 +2769,7 @@
       <c r="A7" s="60">
         <v>5</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="72" t="s">
         <v>145</v>
       </c>
       <c r="C7" s="60" t="s">
@@ -2784,7 +2795,7 @@
       <c r="A8" s="60">
         <v>6</v>
       </c>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="72" t="s">
         <v>150</v>
       </c>
       <c r="C8" s="60" t="s">
@@ -2806,7 +2817,7 @@
       <c r="A9" s="60">
         <v>7</v>
       </c>
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="72" t="s">
         <v>154</v>
       </c>
       <c r="C9" s="60" t="s">
@@ -2841,7 +2852,7 @@
   <dimension ref="A1:AH26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
@@ -2852,8 +2863,8 @@
     <col min="4" max="4" width="12.75" style="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.25" style="26" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="4.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="4.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="7.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="4.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="14" max="19" width="4" style="26" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="4.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="6.33203125" style="26" bestFit="1" customWidth="1"/>
@@ -2934,12 +2945,12 @@
     </row>
     <row r="3" spans="1:34" ht="30.5" thickBot="1">
       <c r="A3" s="27"/>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="73"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
@@ -2972,38 +2983,38 @@
     </row>
     <row r="4" spans="1:34" ht="32">
       <c r="A4" s="27"/>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="78" t="s">
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="82" t="s">
         <v>123</v>
       </c>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="79"/>
-      <c r="T4" s="79"/>
-      <c r="U4" s="80"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="84"/>
       <c r="V4" s="49" t="s">
         <v>88</v>
       </c>
@@ -3013,10 +3024,10 @@
     </row>
     <row r="5" spans="1:34">
       <c r="A5" s="27"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
       <c r="F5" s="32" t="s">
         <v>117</v>
       </c>
@@ -3070,7 +3081,7 @@
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="27"/>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="88" t="s">
         <v>111</v>
       </c>
       <c r="C6" s="33" t="s">
@@ -3105,7 +3116,7 @@
     </row>
     <row r="7" spans="1:34">
       <c r="A7" s="27"/>
-      <c r="B7" s="84"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="33" t="s">
         <v>95</v>
       </c>
@@ -3138,8 +3149,8 @@
     </row>
     <row r="8" spans="1:34">
       <c r="A8" s="27"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="86" t="s">
+      <c r="B8" s="88"/>
+      <c r="C8" s="90" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="33" t="s">
@@ -3171,8 +3182,8 @@
     </row>
     <row r="9" spans="1:34">
       <c r="A9" s="27"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="86"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="90"/>
       <c r="D9" s="33" t="s">
         <v>101</v>
       </c>
@@ -3202,20 +3213,20 @@
     </row>
     <row r="10" spans="1:34">
       <c r="A10" s="27"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="86" t="s">
+      <c r="B10" s="88"/>
+      <c r="C10" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="90" t="s">
         <v>113</v>
       </c>
       <c r="E10" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="94" t="s">
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="70" t="s">
         <v>161</v>
       </c>
       <c r="J10" s="34"/>
@@ -3237,17 +3248,17 @@
     </row>
     <row r="11" spans="1:34">
       <c r="A11" s="27"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
       <c r="E11" s="33" t="s">
         <v>137</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="93"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="69"/>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
       <c r="M11" s="34"/>
@@ -3266,9 +3277,9 @@
     </row>
     <row r="12" spans="1:34">
       <c r="A12" s="27"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="89" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="65" t="s">
         <v>159</v>
       </c>
       <c r="E12" s="62" t="s">
@@ -3276,15 +3287,17 @@
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="93"/>
-      <c r="M12" s="93"/>
-      <c r="N12" s="91"/>
-      <c r="O12" s="91"/>
-      <c r="P12" s="91"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
       <c r="Q12" s="59"/>
       <c r="R12" s="59"/>
       <c r="S12" s="34"/>
@@ -3297,8 +3310,8 @@
     </row>
     <row r="13" spans="1:34">
       <c r="A13" s="27"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="86"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="33" t="s">
         <v>115</v>
       </c>
@@ -3309,7 +3322,7 @@
       <c r="G13" s="34"/>
       <c r="H13" s="59"/>
       <c r="I13" s="59"/>
-      <c r="J13" s="94" t="s">
+      <c r="J13" s="70" t="s">
         <v>162</v>
       </c>
       <c r="K13" s="34"/>
@@ -3330,9 +3343,9 @@
     </row>
     <row r="14" spans="1:34">
       <c r="A14" s="27"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="81" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="85" t="s">
         <v>83</v>
       </c>
       <c r="E14" s="33" t="s">
@@ -3361,9 +3374,9 @@
     </row>
     <row r="15" spans="1:34">
       <c r="A15" s="27"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="82"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="86"/>
       <c r="E15" s="34" t="s">
         <v>138</v>
       </c>
@@ -3378,8 +3391,8 @@
       <c r="N15" s="34"/>
       <c r="O15" s="34"/>
       <c r="P15" s="34"/>
-      <c r="Q15" s="93"/>
-      <c r="R15" s="93"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
       <c r="S15" s="34"/>
       <c r="T15" s="34"/>
       <c r="U15" s="34"/>
@@ -3390,9 +3403,9 @@
     </row>
     <row r="16" spans="1:34">
       <c r="A16" s="27"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="83"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="87"/>
       <c r="E16" s="33" t="s">
         <v>139</v>
       </c>
@@ -3404,7 +3417,7 @@
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
       <c r="M16" s="59"/>
-      <c r="N16" s="88"/>
+      <c r="N16" s="64"/>
       <c r="O16" s="34"/>
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
@@ -3419,11 +3432,11 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="27"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="86" t="s">
+      <c r="B17" s="88"/>
+      <c r="C17" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="86" t="s">
+      <c r="D17" s="90" t="s">
         <v>105</v>
       </c>
       <c r="E17" s="33" t="s">
@@ -3452,9 +3465,9 @@
     </row>
     <row r="18" spans="1:23" ht="17.5" thickBot="1">
       <c r="A18" s="27"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
       <c r="E18" s="54" t="s">
         <v>107</v>
       </c>
@@ -3472,8 +3485,8 @@
       <c r="Q18" s="55"/>
       <c r="R18" s="55"/>
       <c r="S18" s="55"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
+      <c r="T18" s="66"/>
+      <c r="U18" s="66"/>
       <c r="V18" s="56">
         <v>0</v>
       </c>
@@ -3491,7 +3504,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="B21" s="5"/>
-      <c r="T21" s="92"/>
+      <c r="T21" s="68"/>
       <c r="U21" s="44" t="s">
         <v>132</v>
       </c>
@@ -3522,13 +3535,20 @@
       </c>
     </row>
     <row r="25" spans="1:23">
-      <c r="B25" s="5"/>
+      <c r="B25" s="63" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="26" spans="1:23">
       <c r="B26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
     <mergeCell ref="N4:U4"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="B6:B18"/>
@@ -3538,11 +3558,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="F4:M4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix stopu 2022-06-30 추가
</commit_message>
<xml_diff>
--- a/교사팀_기능명세서.xlsx
+++ b/교사팀_기능명세서.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="168">
   <si>
     <t>대분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -695,6 +695,10 @@
   </si>
   <si>
     <t>시도별카테고리 카드섹션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-06-30 버튼생성후 js추가 해결</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1535,27 +1539,6 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1585,6 +1568,27 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1999,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
@@ -2651,7 +2655,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G10" sqref="A1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2887,7 +2891,9 @@
         <v>166</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="18" t="s">
+        <v>167</v>
+      </c>
       <c r="H10" s="18" t="s">
         <v>165</v>
       </c>
@@ -3000,12 +3006,12 @@
     </row>
     <row r="3" spans="1:34" ht="32.25" thickBot="1">
       <c r="A3" s="27"/>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="84"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
@@ -3038,38 +3044,38 @@
     </row>
     <row r="4" spans="1:34" ht="27">
       <c r="A4" s="27"/>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="89" t="s">
+      <c r="F4" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="89" t="s">
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="82" t="s">
         <v>123</v>
       </c>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="91"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="84"/>
       <c r="V4" s="49" t="s">
         <v>88</v>
       </c>
@@ -3079,10 +3085,10 @@
     </row>
     <row r="5" spans="1:34">
       <c r="A5" s="27"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
       <c r="F5" s="32" t="s">
         <v>117</v>
       </c>
@@ -3136,7 +3142,7 @@
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="27"/>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="88" t="s">
         <v>111</v>
       </c>
       <c r="C6" s="33" t="s">
@@ -3171,7 +3177,7 @@
     </row>
     <row r="7" spans="1:34">
       <c r="A7" s="27"/>
-      <c r="B7" s="95"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="33" t="s">
         <v>95</v>
       </c>
@@ -3204,8 +3210,8 @@
     </row>
     <row r="8" spans="1:34">
       <c r="A8" s="27"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="97" t="s">
+      <c r="B8" s="88"/>
+      <c r="C8" s="90" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="33" t="s">
@@ -3237,8 +3243,8 @@
     </row>
     <row r="9" spans="1:34">
       <c r="A9" s="27"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="97"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="90"/>
       <c r="D9" s="33" t="s">
         <v>101</v>
       </c>
@@ -3268,11 +3274,11 @@
     </row>
     <row r="10" spans="1:34">
       <c r="A10" s="27"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="97" t="s">
+      <c r="B10" s="88"/>
+      <c r="C10" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="90" t="s">
         <v>113</v>
       </c>
       <c r="E10" s="33" t="s">
@@ -3303,9 +3309,9 @@
     </row>
     <row r="11" spans="1:34">
       <c r="A11" s="27"/>
-      <c r="B11" s="95"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="97"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
       <c r="E11" s="33" t="s">
         <v>137</v>
       </c>
@@ -3332,8 +3338,8 @@
     </row>
     <row r="12" spans="1:34">
       <c r="A12" s="27"/>
-      <c r="B12" s="95"/>
-      <c r="C12" s="97"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="65" t="s">
         <v>159</v>
       </c>
@@ -3365,8 +3371,8 @@
     </row>
     <row r="13" spans="1:34">
       <c r="A13" s="27"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="97"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="33" t="s">
         <v>115</v>
       </c>
@@ -3398,9 +3404,9 @@
     </row>
     <row r="14" spans="1:34">
       <c r="A14" s="27"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="92" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="85" t="s">
         <v>83</v>
       </c>
       <c r="E14" s="33" t="s">
@@ -3429,9 +3435,9 @@
     </row>
     <row r="15" spans="1:34">
       <c r="A15" s="27"/>
-      <c r="B15" s="95"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="93"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="86"/>
       <c r="E15" s="34" t="s">
         <v>138</v>
       </c>
@@ -3458,9 +3464,9 @@
     </row>
     <row r="16" spans="1:34">
       <c r="A16" s="27"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="94"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="87"/>
       <c r="E16" s="33" t="s">
         <v>139</v>
       </c>
@@ -3487,11 +3493,11 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="27"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="97" t="s">
+      <c r="B17" s="88"/>
+      <c r="C17" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="97" t="s">
+      <c r="D17" s="90" t="s">
         <v>105</v>
       </c>
       <c r="E17" s="33" t="s">
@@ -3520,9 +3526,9 @@
     </row>
     <row r="18" spans="1:23" ht="17.25" thickBot="1">
       <c r="A18" s="27"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="98"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
       <c r="E18" s="54" t="s">
         <v>107</v>
       </c>
@@ -3599,6 +3605,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
     <mergeCell ref="N4:U4"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="B6:B18"/>
@@ -3608,11 +3619,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="F4:M4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix stopu 또 수정
</commit_message>
<xml_diff>
--- a/교사팀_기능명세서.xlsx
+++ b/교사팀_기능명세서.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15615" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15615"/>
   </bookViews>
   <sheets>
     <sheet name="기능명세서" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="171">
   <si>
     <t>대분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -699,6 +699,18 @@
   </si>
   <si>
     <t>2022-06-30 버튼생성후 js추가 해결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발일정 issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능명세서 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>excel다운을 하기 위해서는 jsp로 해야함 jsp는 모든 기능이 완료 된 후로 예정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1292,7 +1304,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1539,6 +1551,27 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1569,26 +1602,8 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2003,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5"/>
@@ -2259,7 +2274,7 @@
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="7">
-        <v>44746</v>
+        <v>44748</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -2533,7 +2548,7 @@
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="7">
-        <v>44748</v>
+        <v>44746</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -2551,7 +2566,7 @@
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="7">
-        <v>44749</v>
+        <v>44747</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -2652,10 +2667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G10" sqref="A1:H10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2664,7 +2679,7 @@
     <col min="2" max="2" width="11.125" style="13" customWidth="1"/>
     <col min="3" max="3" width="14.125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="80.5" bestFit="1" customWidth="1"/>
@@ -2890,13 +2905,42 @@
       <c r="E10" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7">
+        <v>44742</v>
+      </c>
       <c r="G10" s="18" t="s">
         <v>167</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>165</v>
       </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="17">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="7">
+        <v>44742</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F11" s="7">
+        <v>44742</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="E12" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3006,12 +3050,12 @@
     </row>
     <row r="3" spans="1:34" ht="32.25" thickBot="1">
       <c r="A3" s="27"/>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="94"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="84"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
@@ -3044,38 +3088,38 @@
     </row>
     <row r="4" spans="1:34" ht="27">
       <c r="A4" s="27"/>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="82" t="s">
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="89" t="s">
         <v>123</v>
       </c>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="84"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="91"/>
       <c r="V4" s="49" t="s">
         <v>88</v>
       </c>
@@ -3085,10 +3129,10 @@
     </row>
     <row r="5" spans="1:34">
       <c r="A5" s="27"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
       <c r="F5" s="32" t="s">
         <v>117</v>
       </c>
@@ -3142,7 +3186,7 @@
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="27"/>
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="95" t="s">
         <v>111</v>
       </c>
       <c r="C6" s="33" t="s">
@@ -3177,7 +3221,7 @@
     </row>
     <row r="7" spans="1:34">
       <c r="A7" s="27"/>
-      <c r="B7" s="88"/>
+      <c r="B7" s="95"/>
       <c r="C7" s="33" t="s">
         <v>95</v>
       </c>
@@ -3210,8 +3254,8 @@
     </row>
     <row r="8" spans="1:34">
       <c r="A8" s="27"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="90" t="s">
+      <c r="B8" s="95"/>
+      <c r="C8" s="97" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="33" t="s">
@@ -3243,8 +3287,8 @@
     </row>
     <row r="9" spans="1:34">
       <c r="A9" s="27"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="90"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="33" t="s">
         <v>101</v>
       </c>
@@ -3274,11 +3318,11 @@
     </row>
     <row r="10" spans="1:34">
       <c r="A10" s="27"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="90" t="s">
+      <c r="B10" s="95"/>
+      <c r="C10" s="97" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="90" t="s">
+      <c r="D10" s="97" t="s">
         <v>113</v>
       </c>
       <c r="E10" s="33" t="s">
@@ -3309,9 +3353,9 @@
     </row>
     <row r="11" spans="1:34">
       <c r="A11" s="27"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
       <c r="E11" s="33" t="s">
         <v>137</v>
       </c>
@@ -3338,8 +3382,8 @@
     </row>
     <row r="12" spans="1:34">
       <c r="A12" s="27"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="90"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="65" t="s">
         <v>159</v>
       </c>
@@ -3371,8 +3415,8 @@
     </row>
     <row r="13" spans="1:34">
       <c r="A13" s="27"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="90"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="33" t="s">
         <v>115</v>
       </c>
@@ -3404,9 +3448,9 @@
     </row>
     <row r="14" spans="1:34">
       <c r="A14" s="27"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="85" t="s">
+      <c r="B14" s="95"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="92" t="s">
         <v>83</v>
       </c>
       <c r="E14" s="33" t="s">
@@ -3435,9 +3479,9 @@
     </row>
     <row r="15" spans="1:34">
       <c r="A15" s="27"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="86"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="93"/>
       <c r="E15" s="34" t="s">
         <v>138</v>
       </c>
@@ -3464,9 +3508,9 @@
     </row>
     <row r="16" spans="1:34">
       <c r="A16" s="27"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="87"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="94"/>
       <c r="E16" s="33" t="s">
         <v>139</v>
       </c>
@@ -3493,11 +3537,11 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="27"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="90" t="s">
+      <c r="B17" s="95"/>
+      <c r="C17" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="90" t="s">
+      <c r="D17" s="97" t="s">
         <v>105</v>
       </c>
       <c r="E17" s="33" t="s">
@@ -3526,9 +3570,9 @@
     </row>
     <row r="18" spans="1:23" ht="17.25" thickBot="1">
       <c r="A18" s="27"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98"/>
       <c r="E18" s="54" t="s">
         <v>107</v>
       </c>
@@ -3605,11 +3649,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
     <mergeCell ref="N4:U4"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="B6:B18"/>
@@ -3619,6 +3658,11 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="F4:M4"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>